<commit_message>
Add more DRA functionality, clear documentation
</commit_message>
<xml_diff>
--- a/Internship_Survey_OtherResults.xlsx
+++ b/Internship_Survey_OtherResults.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camin\Code\stack_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E2A485-D78C-4527-8CE5-7DC86609B93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F744DC08-B74A-4935-9691-072B4DB66821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{E88566A5-A73A-449C-8D61-F82C95A8D7A3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{E88566A5-A73A-449C-8D61-F82C95A8D7A3}"/>
   </bookViews>
   <sheets>
     <sheet name="InternSwap_Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Hyerim_Survey_Raw" sheetId="2" r:id="rId2"/>
     <sheet name="Internship_Survey_CLEAN" sheetId="3" r:id="rId3"/>
     <sheet name="Data_Summary" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3708" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="212">
   <si>
     <t>J*** S***</t>
   </si>
@@ -645,6 +646,33 @@
   </si>
   <si>
     <t>Not specified</t>
+  </si>
+  <si>
+    <t>Abbreviation name</t>
+  </si>
+  <si>
+    <t>Statistical position</t>
+  </si>
+  <si>
+    <t>Statistical stack</t>
+  </si>
+  <si>
+    <t>Conventional stack</t>
+  </si>
+  <si>
+    <t>Stack position</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>RNS</t>
+  </si>
+  <si>
+    <t>StG</t>
+  </si>
+  <si>
+    <t>JHH</t>
   </si>
 </sst>
 </file>
@@ -804,7 +832,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -840,13 +868,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -857,6 +908,1081 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data_Summary!$Q$19:$Q$28</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>ANU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>James Cook University</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Notre Dame</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UNE/Newcastle</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>UNSW</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Wollongong</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WSU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>USYD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Not specified</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data_Summary!$R$19:$R$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A922-423D-AA4A-832A39594893}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16668</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>26193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>378618</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50006</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DE9D043-D6C7-454B-8E5A-70BF2AA781A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12203,8 +13329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5026BF67-A828-4264-9FCE-3BFC4026A5D0}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12669,7 +13795,7 @@
   <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16558,8 +17684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8CF864-E35C-4756-A3A7-A0E213D726B9}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17395,7 +18521,10 @@
       <c r="R19" s="23">
         <v>1</v>
       </c>
-      <c r="S19" s="4"/>
+      <c r="S19" s="26">
+        <f t="shared" ref="S19:S26" si="2">R19/SUM($R$19:$R$27)</f>
+        <v>2.7247956403269754E-3</v>
+      </c>
       <c r="T19" s="4"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.45">
@@ -17405,6 +18534,10 @@
       <c r="R20" s="13">
         <v>1</v>
       </c>
+      <c r="S20" s="26">
+        <f t="shared" si="2"/>
+        <v>2.7247956403269754E-3</v>
+      </c>
       <c r="T20" s="24"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.45">
@@ -17414,6 +18547,10 @@
       <c r="R21" s="13">
         <v>64</v>
       </c>
+      <c r="S21" s="26">
+        <f t="shared" si="2"/>
+        <v>0.17438692098092642</v>
+      </c>
       <c r="T21" s="24"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.45">
@@ -17423,6 +18560,10 @@
       <c r="R22" s="13">
         <v>15</v>
       </c>
+      <c r="S22" s="26">
+        <f t="shared" si="2"/>
+        <v>4.0871934604904632E-2</v>
+      </c>
       <c r="T22" s="24"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.45">
@@ -17432,6 +18573,10 @@
       <c r="R23" s="13">
         <v>84</v>
       </c>
+      <c r="S23" s="26">
+        <f t="shared" si="2"/>
+        <v>0.22888283378746593</v>
+      </c>
       <c r="T23" s="24"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.45">
@@ -17441,6 +18586,10 @@
       <c r="R24" s="13">
         <v>2</v>
       </c>
+      <c r="S24" s="26">
+        <f t="shared" si="2"/>
+        <v>5.4495912806539508E-3</v>
+      </c>
       <c r="T24" s="24"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.45">
@@ -17450,6 +18599,10 @@
       <c r="R25" s="13">
         <v>18</v>
       </c>
+      <c r="S25" s="26">
+        <f t="shared" si="2"/>
+        <v>4.9046321525885561E-2</v>
+      </c>
       <c r="T25" s="24"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.45">
@@ -17459,6 +18612,10 @@
       <c r="R26" s="13">
         <v>180</v>
       </c>
+      <c r="S26" s="26">
+        <f t="shared" si="2"/>
+        <v>0.49046321525885561</v>
+      </c>
       <c r="T26" s="24"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.45">
@@ -17468,6 +18625,10 @@
       <c r="R27" s="13">
         <v>2</v>
       </c>
+      <c r="S27" s="26">
+        <f>R27/SUM($R$19:$R$27)</f>
+        <v>5.4495912806539508E-3</v>
+      </c>
       <c r="T27" s="24"/>
     </row>
     <row r="28" spans="2:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -17478,6 +18639,7 @@
         <f>SUM(R19:R27)</f>
         <v>367</v>
       </c>
+      <c r="S28" s="25"/>
       <c r="T28" s="24"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.45">
@@ -17499,6 +18661,635 @@
       <c r="T34" s="24"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4D1976-B388-4C3F-8F20-0A1E4752E0C5}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2</f>
+        <v>RNS</v>
+      </c>
+      <c r="H2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>VLOOKUP(H2,$E$2:F16,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f>J2-I2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.54761904761904767</v>
+      </c>
+      <c r="E3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G16" si="0">E3</f>
+        <v>RPA</v>
+      </c>
+      <c r="H3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f>VLOOKUP(H3,$E$2:F17,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K16" si="1">J3-I3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Concord</v>
+      </c>
+      <c r="H4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f>VLOOKUP(H4,$E$2:F18,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>POW</v>
+      </c>
+      <c r="H5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <f>VLOOKUP(H5,$E$2:F19,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.72413793103448276</v>
+      </c>
+      <c r="E6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>StV</v>
+      </c>
+      <c r="H6" t="s">
+        <v>190</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f>VLOOKUP(H6,$E$2:F20,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>StG</v>
+      </c>
+      <c r="H7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f>VLOOKUP(H7,$E$2:F21,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Hornsby</v>
+      </c>
+      <c r="H8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <f>VLOOKUP(H8,$E$2:F22,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.3666666666666667</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Westmead</v>
+      </c>
+      <c r="H9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <f>VLOOKUP(H9,$E$2:F23,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1.5294117647058822</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Liverpool</v>
+      </c>
+      <c r="H10" t="s">
+        <v>211</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <f>VLOOKUP(H10,$E$2:F24,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1.7647058823529411</v>
+      </c>
+      <c r="E11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Gosford</v>
+      </c>
+      <c r="H11" t="s">
+        <v>191</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <f>VLOOKUP(H11,$E$2:F25,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.7647058823529411</v>
+      </c>
+      <c r="E12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>JHH</v>
+      </c>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <f>VLOOKUP(H12,$E$2:F26,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.8461538461538463</v>
+      </c>
+      <c r="E13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Nepean</v>
+      </c>
+      <c r="H13" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <f>VLOOKUP(H13,$E$2:F27,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15">
+        <v>2.75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>Wollongong</v>
+      </c>
+      <c r="H14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <f>VLOOKUP(H14,$E$2:F28,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>Blacktown</v>
+      </c>
+      <c r="H15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <f>VLOOKUP(H15,$E$2:F29,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="17">
+        <v>2</v>
+      </c>
+      <c r="C16" s="17">
+        <v>14</v>
+      </c>
+      <c r="D16" s="20">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>Bankstown</v>
+      </c>
+      <c r="H16" t="s">
+        <v>201</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <f>VLOOKUP(H16,$E$2:F30,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K2:K16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major bugfix (stack with random elements now uses stack) and implementation of alternative stack
</commit_message>
<xml_diff>
--- a/Internship_Survey_OtherResults.xlsx
+++ b/Internship_Survey_OtherResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camin\Code\stack_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F744DC08-B74A-4935-9691-072B4DB66821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31990000-93DC-4199-9B27-1AF9C571913C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{E88566A5-A73A-449C-8D61-F82C95A8D7A3}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Data_Summary" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$Q$1:$R$16</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3821" uniqueCount="224">
   <si>
     <t>J*** S***</t>
   </si>
@@ -673,6 +676,42 @@
   </si>
   <si>
     <t>JHH</t>
+  </si>
+  <si>
+    <t>Arithmetic average position</t>
+  </si>
+  <si>
+    <t>Geometric average position</t>
+  </si>
+  <si>
+    <t>aavpos</t>
+  </si>
+  <si>
+    <t>Arithmetic position</t>
+  </si>
+  <si>
+    <t>gavpos</t>
+  </si>
+  <si>
+    <t>Geometric position</t>
+  </si>
+  <si>
+    <t>Arithmetic compromise stack</t>
+  </si>
+  <si>
+    <t>Geometric compromise stack</t>
+  </si>
+  <si>
+    <t>Harmonic compromise stack</t>
+  </si>
+  <si>
+    <t>Harmonic average position</t>
+  </si>
+  <si>
+    <t>havpos</t>
+  </si>
+  <si>
+    <t>Harmonic position</t>
   </si>
 </sst>
 </file>
@@ -879,21 +918,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1020,6 +1059,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1040,6 +1084,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1060,6 +1109,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1080,6 +1134,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1100,6 +1159,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1120,6 +1184,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1142,6 +1211,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1164,6 +1238,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1186,6 +1265,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1208,6 +1292,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-2D58-4CC7-B501-5D60CA37120A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2284,9 +2373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887A97C5-7889-4D3E-AB7B-4D0AB39440E0}">
   <dimension ref="A1:D920"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -13794,9 +13881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BDC4F8-2455-4A67-AC08-7722B5EEEFD6}">
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -17684,8 +17769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8CF864-E35C-4756-A3A7-A0E213D726B9}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18668,15 +18753,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4D1976-B388-4C3F-8F20-0A1E4752E0C5}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="18" max="20" width="9.06640625" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="9.06640625" customWidth="1"/>
+    <col min="24" max="26" width="9.06640625" hidden="1" customWidth="1"/>
+    <col min="30" max="32" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>183</v>
       </c>
@@ -18695,23 +18786,67 @@
       <c r="F1" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>131</v>
       </c>
@@ -18730,26 +18865,77 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <f>E2</f>
         <v>RNS</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>188</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <f>VLOOKUP(H2,$E$2:F16,2,FALSE)</f>
+      <c r="K2">
+        <f>VLOOKUP(I2,$E$2:F16,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="K2">
-        <f>J2-I2</f>
+      <c r="L2">
+        <f>K2-J2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M2">
+        <f>AVERAGE(J2:K2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N2">
+        <f>SQRT(J2*K2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O2">
+        <f>2/(1/J2+1/K2)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>188</v>
+      </c>
+      <c r="R2">
+        <v>1.5</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="str">
+        <f>T2&amp;S2</f>
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>188</v>
+      </c>
+      <c r="X2">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="str">
+        <f>Z2&amp;Y2</f>
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD2">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="str">
+        <f>AF2&amp;AE2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>132</v>
       </c>
@@ -18768,26 +18954,92 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G16" si="0">E3</f>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H16" si="0">E3</f>
         <v>RPA</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>209</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <f>VLOOKUP(H3,$E$2:F17,2,FALSE)</f>
+      <c r="K3">
+        <f>VLOOKUP(I3,$E$2:F17,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K16" si="1">J3-I3</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L16" si="1">K3-J3</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M3">
+        <f t="shared" ref="M3:M16" si="2">AVERAGE(J3:K3)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N16" si="3">SQRT(J3*K3)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O16" si="4">2/(1/J3+1/K3)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>209</v>
+      </c>
+      <c r="R3">
+        <v>1.5</v>
+      </c>
+      <c r="S3">
+        <f>IF(R3&gt;R2,S2+1,S2)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" t="str">
+        <f>IF(S3=S2,"=", "")</f>
+        <v>=</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U16" si="5">T3&amp;S3</f>
+        <v>=1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>209</v>
+      </c>
+      <c r="X3">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Y3">
+        <f>IF(X3&gt;X2,Y2+1,Y2)</f>
+        <v>1</v>
+      </c>
+      <c r="Z3" t="str">
+        <f>IF(Y3=Y2,"=", "")</f>
+        <v>=</v>
+      </c>
+      <c r="AA3" t="str">
+        <f t="shared" ref="AA3:AA16" si="6">Z3&amp;Y3</f>
+        <v>=1</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD3">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="AE3">
+        <f>IF(AD3&gt;AD2,AE2+1,AE2)</f>
+        <v>1</v>
+      </c>
+      <c r="AF3" t="str">
+        <f>IF(AE3=AE2,"=", "")</f>
+        <v>=</v>
+      </c>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG16" si="7">AF3&amp;AE3</f>
+        <v>=1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>136</v>
       </c>
@@ -18806,26 +19058,92 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>Concord</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>196</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
-        <f>VLOOKUP(H4,$E$2:F18,2,FALSE)</f>
+      <c r="K4">
+        <f>VLOOKUP(I4,$E$2:F18,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>3.4285714285714288</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>196</v>
+      </c>
+      <c r="R4">
+        <v>3.5</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S16" si="8">IF(R4&gt;R3,S3+1,S3)</f>
+        <v>2</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" ref="T4:T16" si="9">IF(S4=S3,"=", "")</f>
+        <v/>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="W4" t="s">
+        <v>196</v>
+      </c>
+      <c r="X4">
+        <v>3.4641016151377544</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y16" si="10">IF(X4&gt;X3,Y3+1,Y3)</f>
+        <v>2</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" ref="Z4:Z16" si="11">IF(Y4=Y3,"=", "")</f>
+        <v/>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD4">
+        <v>3.4285714285714288</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" ref="AE4:AE16" si="12">IF(AD4&gt;AD3,AE3+1,AE3)</f>
+        <v>2</v>
+      </c>
+      <c r="AF4" t="str">
+        <f t="shared" ref="AF4:AF16" si="13">IF(AE4=AE3,"=", "")</f>
+        <v/>
+      </c>
+      <c r="AG4" t="str">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>133</v>
       </c>
@@ -18844,26 +19162,92 @@
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>POW</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>197</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="J5">
-        <f>VLOOKUP(H5,$E$2:F19,2,FALSE)</f>
+      <c r="K5">
+        <f>VLOOKUP(I5,$E$2:F19,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>190</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="W5" t="s">
+        <v>190</v>
+      </c>
+      <c r="X5">
+        <v>3.872983346207417</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="Z5" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD5">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="AF5" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG5" t="str">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>134</v>
       </c>
@@ -18882,26 +19266,92 @@
       <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>StV</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>190</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <f>VLOOKUP(H6,$E$2:F20,2,FALSE)</f>
+      <c r="K6">
+        <f>VLOOKUP(I6,$E$2:F20,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>3.872983346207417</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>3.75</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>197</v>
+      </c>
+      <c r="R6">
+        <v>4.5</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="W6" t="s">
+        <v>197</v>
+      </c>
+      <c r="X6">
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD6">
+        <v>3.75</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="AF6" t="str">
+        <f t="shared" si="13"/>
+        <v>=</v>
+      </c>
+      <c r="AG6" t="str">
+        <f t="shared" si="7"/>
+        <v>=3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>135</v>
       </c>
@@ -18920,26 +19370,92 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>StG</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>210</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7">
-        <f>VLOOKUP(H7,$E$2:F21,2,FALSE)</f>
+      <c r="K7">
+        <f>VLOOKUP(I7,$E$2:F21,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>210</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="W7" t="s">
+        <v>210</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD7">
+        <v>6</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="AF7" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG7" t="str">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>137</v>
       </c>
@@ -18958,26 +19474,92 @@
       <c r="F8">
         <v>7</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>Hornsby</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>199</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>7</v>
       </c>
-      <c r="J8">
-        <f>VLOOKUP(H8,$E$2:F22,2,FALSE)</f>
-        <v>8</v>
-      </c>
       <c r="K8">
+        <f>VLOOKUP(I8,$E$2:F22,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>7.4833147735478827</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>7.4666666666666668</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>199</v>
+      </c>
+      <c r="R8">
+        <v>7.5</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="W8" t="s">
+        <v>199</v>
+      </c>
+      <c r="X8">
+        <v>7.4833147735478827</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD8">
+        <v>7.4666666666666668</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="AF8" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG8" t="str">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>138</v>
       </c>
@@ -18996,26 +19578,92 @@
       <c r="F9">
         <v>8</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>Westmead</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>193</v>
       </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
       <c r="J9">
-        <f>VLOOKUP(H9,$E$2:F23,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f>VLOOKUP(I9,$E$2:F23,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>7.4833147735478827</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>7.4666666666666668</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>193</v>
+      </c>
+      <c r="R9">
+        <v>7.5</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="9"/>
+        <v>=</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="5"/>
+        <v>=6</v>
+      </c>
+      <c r="W9" t="s">
+        <v>193</v>
+      </c>
+      <c r="X9">
+        <v>7.4833147735478827</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="11"/>
+        <v>=</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="6"/>
+        <v>=6</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD9">
+        <v>7.4666666666666668</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="AF9" t="str">
+        <f t="shared" si="13"/>
+        <v>=</v>
+      </c>
+      <c r="AG9" t="str">
+        <f t="shared" si="7"/>
+        <v>=5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>139</v>
       </c>
@@ -19034,26 +19682,92 @@
       <c r="F10">
         <v>9</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>Liverpool</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>211</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>9</v>
       </c>
-      <c r="J10">
-        <f>VLOOKUP(H10,$E$2:F24,2,FALSE)</f>
+      <c r="K10">
+        <f>VLOOKUP(I10,$E$2:F24,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>9.9498743710661994</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>9.9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>191</v>
+      </c>
+      <c r="R10">
+        <v>9.5</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="W10" t="s">
+        <v>191</v>
+      </c>
+      <c r="X10">
+        <v>9.4868329805051381</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD10">
+        <v>9.9</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="AF10" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG10" t="str">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>141</v>
       </c>
@@ -19072,26 +19786,92 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>Gosford</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>191</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>10</v>
       </c>
-      <c r="J11">
-        <f>VLOOKUP(H11,$E$2:F25,2,FALSE)</f>
+      <c r="K11">
+        <f>VLOOKUP(I11,$E$2:F25,2,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>9.4868329805051381</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>9.473684210526315</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>211</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="W11" t="s">
+        <v>211</v>
+      </c>
+      <c r="X11">
+        <v>9.9498743710661994</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD11">
+        <v>9.473684210526315</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="AF11" t="str">
+        <f t="shared" si="13"/>
+        <v>=</v>
+      </c>
+      <c r="AG11" t="str">
+        <f t="shared" si="7"/>
+        <v>=6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>140</v>
       </c>
@@ -19110,26 +19890,92 @@
       <c r="F12">
         <v>11</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>JHH</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>189</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>11</v>
       </c>
-      <c r="J12">
-        <f>VLOOKUP(H12,$E$2:F26,2,FALSE)</f>
+      <c r="K12">
+        <f>VLOOKUP(I12,$E$2:F26,2,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>12.845232578665129</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>12.692307692307692</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>194</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="W12" t="s">
+        <v>194</v>
+      </c>
+      <c r="X12">
+        <v>10.954451150103322</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="Z12" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD12">
+        <v>12.692307692307692</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="AF12" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG12" t="str">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>144</v>
       </c>
@@ -19148,26 +19994,92 @@
       <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>Nepean</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>194</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>12</v>
       </c>
-      <c r="J13">
-        <f>VLOOKUP(H13,$E$2:F27,2,FALSE)</f>
+      <c r="K13">
+        <f>VLOOKUP(I13,$E$2:F27,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>10.954451150103322</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>10.909090909090908</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>189</v>
+      </c>
+      <c r="R13">
+        <v>13</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="W13" t="s">
+        <v>189</v>
+      </c>
+      <c r="X13">
+        <v>12.845232578665129</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="Z13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>194</v>
+      </c>
+      <c r="AD13">
+        <v>10.909090909090908</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="AF13" t="str">
+        <f t="shared" si="13"/>
+        <v>=</v>
+      </c>
+      <c r="AG13" t="str">
+        <f t="shared" si="7"/>
+        <v>=7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>143</v>
       </c>
@@ -19186,26 +20098,92 @@
       <c r="F14">
         <v>13</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>Wollongong</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>170</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>13</v>
       </c>
-      <c r="J14">
-        <f>VLOOKUP(H14,$E$2:F28,2,FALSE)</f>
+      <c r="K14">
+        <f>VLOOKUP(I14,$E$2:F28,2,FALSE)</f>
         <v>13</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>170</v>
+      </c>
+      <c r="R14">
+        <v>13</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="9"/>
+        <v>=</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="5"/>
+        <v>=10</v>
+      </c>
+      <c r="W14" t="s">
+        <v>200</v>
+      </c>
+      <c r="X14">
+        <v>12.961481396815721</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="Z14" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD14">
+        <v>13</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="AF14" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG14" t="str">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>145</v>
       </c>
@@ -19224,26 +20202,92 @@
       <c r="F15">
         <v>14</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>Blacktown</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>200</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>14</v>
       </c>
-      <c r="J15">
-        <f>VLOOKUP(H15,$E$2:F29,2,FALSE)</f>
+      <c r="K15">
+        <f>VLOOKUP(I15,$E$2:F29,2,FALSE)</f>
         <v>12</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>12.961481396815721</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>12.923076923076923</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>200</v>
+      </c>
+      <c r="R15">
+        <v>13</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="9"/>
+        <v>=</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="5"/>
+        <v>=10</v>
+      </c>
+      <c r="W15" t="s">
+        <v>170</v>
+      </c>
+      <c r="X15">
+        <v>13</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="Z15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA15" t="str">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD15">
+        <v>12.923076923076923</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="AF15" t="str">
+        <f t="shared" si="13"/>
+        <v>=</v>
+      </c>
+      <c r="AG15" t="str">
+        <f t="shared" si="7"/>
+        <v>=8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="19" t="s">
         <v>142</v>
       </c>
@@ -19262,34 +20306,109 @@
       <c r="F16">
         <v>15</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>Bankstown</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>201</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>15</v>
       </c>
-      <c r="J16">
-        <f>VLOOKUP(H16,$E$2:F30,2,FALSE)</f>
+      <c r="K16">
+        <f>VLOOKUP(I16,$E$2:F30,2,FALSE)</f>
         <v>14</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>14.491376746189438</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>14.482758620689655</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>201</v>
+      </c>
+      <c r="R16">
+        <v>14.5</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="W16" t="s">
+        <v>201</v>
+      </c>
+      <c r="X16">
+        <v>14.491376746189438</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="Z16" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD16">
+        <v>14.482758620689655</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="AF16" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG16" t="str">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <autoFilter ref="Q1:R16" xr:uid="{71D4FD0E-D4F0-4960-B0D6-C600C89A82D3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q2:R16">
+      <sortCondition ref="R2:R16"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="W2:Y16">
+    <sortCondition ref="X2:X16"/>
+  </sortState>
+  <conditionalFormatting sqref="L2:L16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>